<commit_message>
Added  multiple link test
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14970" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12570" windowHeight="6330"/>
   </bookViews>
   <sheets>
     <sheet name="loginTest" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="bookingTest" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O21"/>
+  <oleSize ref="A1:L19"/>
 </workbook>
 </file>
 
@@ -38,8 +38,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -67,8 +75,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,23 +382,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -397,7 +406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -405,7 +414,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -415,6 +424,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated framework to run tests in parallel,added browser factory and updated chrome driver 2.28
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12570" windowHeight="6330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14970" windowHeight="5760"/>
   </bookViews>
   <sheets>
     <sheet name="loginTest" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="3">
   <si>
     <t>username</t>
   </si>
@@ -26,12 +26,6 @@
   </si>
   <si>
     <t>satya</t>
-  </si>
-  <si>
-    <t>james</t>
-  </si>
-  <si>
-    <t>test</t>
   </si>
 </sst>
 </file>
@@ -385,7 +379,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,18 +402,18 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>